<commit_message>
Updated Timeline and Effort Matrix
</commit_message>
<xml_diff>
--- a/Tasks, Milestones, Timeline, Effort Matrix/Timline_EffortMatrix.xlsx
+++ b/Tasks, Milestones, Timeline, Effort Matrix/Timline_EffortMatrix.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Google Drive\UC\2178\CS5001_SeniorDesignI_001\Assignments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam Karrasch\Documents\GitHub\CS_SeniorDesign\Tasks, Milestones, Timeline, Effort Matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Timeline" sheetId="1" r:id="rId1"/>
     <sheet name="EffortMatrix" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
   <si>
     <t>Start Date</t>
   </si>
@@ -103,12 +103,15 @@
   </si>
   <si>
     <t>Ryan</t>
+  </si>
+  <si>
+    <t>Test Application</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -180,11 +183,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,10 +502,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -590,79 +595,79 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B8" s="3">
-        <v>43108</v>
+        <v>43115</v>
       </c>
       <c r="C8" s="3">
-        <v>43140</v>
+        <v>43118</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="B9" s="3">
+        <v>43115</v>
       </c>
       <c r="C9" s="3">
-        <v>43140</v>
+        <v>43122</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="3">
-        <v>43147</v>
+        <v>43108</v>
       </c>
       <c r="C10" s="3">
-        <v>43152</v>
+        <v>43140</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="3">
-        <v>43152</v>
+        <v>43140</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="3">
-        <v>43153</v>
+        <v>43147</v>
       </c>
       <c r="C12" s="3">
-        <v>43158</v>
+        <v>43152</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="3">
-        <v>43153</v>
+        <v>17</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="C13" s="3">
-        <v>43160</v>
+        <v>43152</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B14" s="3">
         <v>43153</v>
       </c>
       <c r="C14" s="3">
-        <v>43160</v>
+        <v>43158</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -705,41 +710,43 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -759,7 +766,7 @@
       <c r="E3" s="5">
         <v>0.2</v>
       </c>
-      <c r="G3" s="8"/>
+      <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -777,7 +784,7 @@
       <c r="E4" s="5">
         <v>0.1</v>
       </c>
-      <c r="G4" s="8"/>
+      <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -795,7 +802,7 @@
       <c r="E5" s="5">
         <v>0.7</v>
       </c>
-      <c r="G5" s="8"/>
+      <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -813,86 +820,86 @@
       <c r="E6" s="5">
         <v>0</v>
       </c>
-      <c r="G6" s="8"/>
+      <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="5">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="C7" s="5">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="5">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="E7" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="G7" s="8"/>
+        <v>0.6</v>
+      </c>
+      <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" s="5">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="C8" s="5">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="D8" s="5">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="E8" s="5">
-        <v>0.6</v>
-      </c>
-      <c r="G8" s="8"/>
+        <v>0.25</v>
+      </c>
+      <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B9" s="5">
-        <v>0.1</v>
+        <v>0.7</v>
       </c>
       <c r="C9" s="5">
         <v>0.1</v>
       </c>
       <c r="D9" s="5">
-        <v>0.7</v>
+        <v>0.1</v>
       </c>
       <c r="E9" s="5">
         <v>0.1</v>
       </c>
-      <c r="G9" s="8"/>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="5">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="C10" s="5">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="D10" s="5">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E10" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="G10" s="8"/>
+        <v>0.2</v>
+      </c>
+      <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" s="5">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="C11" s="5">
         <v>0.2</v>
@@ -901,45 +908,49 @@
         <v>0.2</v>
       </c>
       <c r="E11" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="G11" s="8"/>
+        <v>0.4</v>
+      </c>
+      <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" s="5">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="C12" s="5">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D12" s="5">
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
       <c r="E12" s="5">
-        <v>0.4</v>
-      </c>
-      <c r="G12" s="8"/>
+        <v>0.1</v>
+      </c>
+      <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="C13" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="D13" s="5">
-        <v>0.7</v>
-      </c>
-      <c r="E13" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="G13" s="8"/>
+      <c r="B13" s="7">
+        <f>SUM(B3:B12)</f>
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="C13" s="7">
+        <f>SUM(C3:C12)</f>
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="D13" s="7">
+        <f>SUM(D3:D12)</f>
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="E13" s="7">
+        <f>SUM(E3:E12)</f>
+        <v>2.6500000000000004</v>
+      </c>
+      <c r="F13" s="7">
+        <f>SUM(B13:E13)</f>
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>